<commit_message>
Fix[ITE2]: general fixes on table creations
</commit_message>
<xml_diff>
--- a/proyecto/iteración-2/docs/modelos/modelo-relacional.xlsx
+++ b/proyecto/iteración-2/docs/modelos/modelo-relacional.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zejiran/hack/uniandes/B-03/proyecto/iteración-2/modelos/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zejiran/hack/uniandes/B-03/proyecto/iteración-2/docs/modelos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DE2F519-6D7A-B042-8DB9-2D9577A98590}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27B64E3B-D854-0545-BDDB-BC55207BD12C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="105">
   <si>
     <t>NN</t>
   </si>
@@ -238,18 +238,12 @@
     <t>NN, CK in ('Bodega', 'LocalVentas', 'Estante')</t>
   </si>
   <si>
-    <t>NN, CK in ('PagueLleveUnidad', 'DescuentoPorcentaje', 'PagueLleveCantidad', 'Pague1LleveDescuento2', 'Combo')</t>
-  </si>
-  <si>
     <t>NN, CK in ('CREADA', 'PAGADA', 'CANCELADA')</t>
   </si>
   <si>
     <t>NN, CK in ('gr', 'ml')</t>
   </si>
   <si>
-    <t>NN, CK in ('volumenCm3', 'pesoGR')</t>
-  </si>
-  <si>
     <t>CK in ('PersonaNatural', 'Empresa')</t>
   </si>
   <si>
@@ -332,6 +326,30 @@
   </si>
   <si>
     <t>PK, FK Compra.id</t>
+  </si>
+  <si>
+    <t>NN, CK in F</t>
+  </si>
+  <si>
+    <t>idProducto</t>
+  </si>
+  <si>
+    <t>idProveedor</t>
+  </si>
+  <si>
+    <t>idPedido</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NN, CK in  </t>
+  </si>
+  <si>
+    <t>idSucursal</t>
+  </si>
+  <si>
+    <t>idCompra</t>
+  </si>
+  <si>
+    <t>O</t>
   </si>
 </sst>
 </file>
@@ -868,8 +886,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:L45"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="56" zoomScaleNormal="84" workbookViewId="0">
-      <selection activeCell="K39" sqref="K39"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A9" zoomScale="75" zoomScaleNormal="135" workbookViewId="0">
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -916,19 +934,19 @@
         <v>45</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>79</v>
+        <v>100</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>83</v>
+        <v>102</v>
       </c>
       <c r="J3" s="8" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="K3" s="8" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="L3" s="8" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="4" spans="2:12" s="5" customFormat="1" ht="51" x14ac:dyDescent="0.2">
@@ -949,19 +967,19 @@
       </c>
       <c r="G4" s="9"/>
       <c r="H4" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="I4" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="I4" s="12" t="s">
-        <v>84</v>
-      </c>
       <c r="J4" s="9" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="K4" s="9" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="L4" s="9" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.2">
@@ -996,13 +1014,13 @@
         <v>40</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="G8" s="8" t="s">
-        <v>80</v>
+        <v>98</v>
       </c>
       <c r="I8" s="3" t="s">
         <v>2</v>
@@ -1025,7 +1043,7 @@
         <v>5</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>67</v>
+        <v>97</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>0</v>
@@ -1034,13 +1052,13 @@
         <v>0</v>
       </c>
       <c r="G9" s="12" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="I9" s="4" t="s">
         <v>4</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="K9" s="4" t="s">
         <v>0</v>
@@ -1063,7 +1081,7 @@
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="H12" s="1" t="s">
         <v>9</v>
@@ -1101,7 +1119,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="2:12" ht="34" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:12" ht="17" x14ac:dyDescent="0.2">
       <c r="B14" s="4" t="s">
         <v>4</v>
       </c>
@@ -1124,13 +1142,13 @@
         <v>0</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K14" s="4" t="s">
         <v>0</v>
       </c>
       <c r="L14" s="9" t="s">
-        <v>70</v>
+        <v>101</v>
       </c>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.2">
@@ -1150,10 +1168,10 @@
         <v>8</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="18" spans="2:12" x14ac:dyDescent="0.2">
@@ -1170,19 +1188,22 @@
         <v>34</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="H18" s="8" t="s">
-        <v>8</v>
+        <v>103</v>
       </c>
       <c r="I18" s="8" t="s">
-        <v>80</v>
+        <v>98</v>
+      </c>
+      <c r="J18" s="2" t="s">
+        <v>104</v>
       </c>
       <c r="K18" s="3" t="s">
-        <v>79</v>
+        <v>100</v>
       </c>
       <c r="L18" s="3" t="s">
-        <v>74</v>
+        <v>99</v>
       </c>
     </row>
     <row r="19" spans="2:12" ht="34" x14ac:dyDescent="0.2">
@@ -1194,22 +1215,22 @@
       </c>
       <c r="D19" s="4"/>
       <c r="E19" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F19" s="12" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="H19" s="12" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="I19" s="12" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="K19" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="L19" s="12" t="s">
         <v>76</v>
-      </c>
-      <c r="L19" s="12" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="20" spans="2:12" x14ac:dyDescent="0.2">
@@ -1257,7 +1278,7 @@
         <v>24</v>
       </c>
       <c r="K23" s="8" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="24" spans="2:12" ht="68" x14ac:dyDescent="0.2">
@@ -1268,7 +1289,7 @@
         <v>0</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E24" s="4" t="s">
         <v>0</v>
@@ -1280,12 +1301,12 @@
         <v>0</v>
       </c>
       <c r="H24" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="I24" s="4"/>
       <c r="J24" s="4"/>
       <c r="K24" s="9" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="25" spans="2:12" x14ac:dyDescent="0.2">
@@ -1325,7 +1346,7 @@
         <v>49</v>
       </c>
       <c r="H28" s="3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="29" spans="2:12" ht="68" x14ac:dyDescent="0.2">
@@ -1346,7 +1367,7 @@
       </c>
       <c r="G29" s="9"/>
       <c r="H29" s="12" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="30" spans="2:12" x14ac:dyDescent="0.2">
@@ -1461,7 +1482,7 @@
         <v>61</v>
       </c>
       <c r="I38" s="3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="39" spans="2:11" ht="51" x14ac:dyDescent="0.2">
@@ -1485,7 +1506,7 @@
         <v>63</v>
       </c>
       <c r="I39" s="12" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="40" spans="2:11" x14ac:dyDescent="0.2">
@@ -1503,7 +1524,7 @@
         <v>15</v>
       </c>
       <c r="H42" s="13" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="I42" s="11"/>
     </row>
@@ -1518,16 +1539,16 @@
         <v>54</v>
       </c>
       <c r="E43" s="8" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F43" s="8" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="H43" s="8" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="I43" s="8" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="44" spans="2:11" ht="34" x14ac:dyDescent="0.2">
@@ -1537,16 +1558,16 @@
       <c r="C44" s="4"/>
       <c r="D44" s="4"/>
       <c r="E44" s="9" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F44" s="9" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="H44" s="12" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="I44" s="12" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="45" spans="2:11" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Fix[ITE2]: change table constraints creation
</commit_message>
<xml_diff>
--- a/proyecto/iteración-2/docs/modelos/modelo-relacional.xlsx
+++ b/proyecto/iteración-2/docs/modelos/modelo-relacional.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zejiran/hack/uniandes/B-03/proyecto/iteración-2/docs/modelos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27B64E3B-D854-0545-BDDB-BC55207BD12C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79B732D6-C5AD-D942-B354-870954ED58F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="104">
   <si>
     <t>NN</t>
   </si>
@@ -278,9 +278,6 @@
   </si>
   <si>
     <t>NN, FK Pedido.id</t>
-  </si>
-  <si>
-    <t>sucursal</t>
   </si>
   <si>
     <t>NN, FK Sucursal.id</t>
@@ -886,8 +883,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:L45"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A9" zoomScale="75" zoomScaleNormal="135" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" zoomScale="75" zoomScaleNormal="135" workbookViewId="0">
+      <selection activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -934,19 +931,19 @@
         <v>45</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="J3" s="8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="K3" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="L3" s="8" t="s">
         <v>89</v>
-      </c>
-      <c r="L3" s="8" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="4" spans="2:12" s="5" customFormat="1" ht="51" x14ac:dyDescent="0.2">
@@ -970,16 +967,16 @@
         <v>80</v>
       </c>
       <c r="I4" s="12" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J4" s="9" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="K4" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="L4" s="9" t="s">
         <v>87</v>
-      </c>
-      <c r="L4" s="9" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.2">
@@ -1014,13 +1011,13 @@
         <v>40</v>
       </c>
       <c r="E8" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="F8" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="F8" s="3" t="s">
-        <v>84</v>
-      </c>
       <c r="G8" s="8" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I8" s="3" t="s">
         <v>2</v>
@@ -1043,7 +1040,7 @@
         <v>5</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>0</v>
@@ -1081,7 +1078,7 @@
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H12" s="1" t="s">
         <v>9</v>
@@ -1148,7 +1145,7 @@
         <v>0</v>
       </c>
       <c r="L14" s="9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.2">
@@ -1168,7 +1165,7 @@
         <v>8</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="K17" s="1" t="s">
         <v>73</v>
@@ -1188,22 +1185,22 @@
         <v>34</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H18" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="I18" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="J18" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="I18" s="8" t="s">
+      <c r="K18" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="L18" s="3" t="s">
         <v>98</v>
-      </c>
-      <c r="J18" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="K18" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="L18" s="3" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="19" spans="2:12" ht="34" x14ac:dyDescent="0.2">
@@ -1218,10 +1215,10 @@
         <v>67</v>
       </c>
       <c r="F19" s="12" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H19" s="12" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="I19" s="12" t="s">
         <v>79</v>
@@ -1278,7 +1275,7 @@
         <v>24</v>
       </c>
       <c r="K23" s="8" t="s">
-        <v>81</v>
+        <v>101</v>
       </c>
     </row>
     <row r="24" spans="2:12" ht="68" x14ac:dyDescent="0.2">
@@ -1306,7 +1303,7 @@
       <c r="I24" s="4"/>
       <c r="J24" s="4"/>
       <c r="K24" s="9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="25" spans="2:12" x14ac:dyDescent="0.2">
@@ -1346,10 +1343,10 @@
         <v>49</v>
       </c>
       <c r="H28" s="3" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="29" spans="2:12" ht="68" x14ac:dyDescent="0.2">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="29" spans="2:12" ht="51" x14ac:dyDescent="0.2">
       <c r="B29" s="4" t="s">
         <v>4</v>
       </c>
@@ -1367,7 +1364,7 @@
       </c>
       <c r="G29" s="9"/>
       <c r="H29" s="12" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="30" spans="2:12" x14ac:dyDescent="0.2">
@@ -1482,7 +1479,7 @@
         <v>61</v>
       </c>
       <c r="I38" s="3" t="s">
-        <v>81</v>
+        <v>101</v>
       </c>
     </row>
     <row r="39" spans="2:11" ht="51" x14ac:dyDescent="0.2">
@@ -1506,7 +1503,7 @@
         <v>63</v>
       </c>
       <c r="I39" s="12" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="40" spans="2:11" x14ac:dyDescent="0.2">
@@ -1551,7 +1548,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="44" spans="2:11" ht="34" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:11" ht="17" x14ac:dyDescent="0.2">
       <c r="B44" s="12" t="s">
         <v>4</v>
       </c>
@@ -1561,7 +1558,7 @@
         <v>80</v>
       </c>
       <c r="F44" s="9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H44" s="12" t="s">
         <v>76</v>

</xml_diff>

<commit_message>
Fix: update create proveedor constraints
</commit_message>
<xml_diff>
--- a/proyecto/iteración-2/docs/modelos/modelo-relacional.xlsx
+++ b/proyecto/iteración-2/docs/modelos/modelo-relacional.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10911"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11011"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zejiran/hack/uniandes/B-03/proyecto/iteración-2/docs/modelos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79B732D6-C5AD-D942-B354-870954ED58F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FBAB829-516C-0B4F-BEFA-F7C1EA4F5D92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="105">
   <si>
     <t>NN</t>
   </si>
@@ -347,6 +347,9 @@
   </si>
   <si>
     <t>O</t>
+  </si>
+  <si>
+    <t>DD, CK between 0 and 5</t>
   </si>
 </sst>
 </file>
@@ -883,8 +886,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:L45"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" zoomScale="75" zoomScaleNormal="135" workbookViewId="0">
-      <selection activeCell="I29" sqref="I29"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="75" zoomScaleNormal="135" workbookViewId="0">
+      <selection activeCell="K29" sqref="K29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1437,7 +1440,7 @@
         <v>0</v>
       </c>
       <c r="K34" s="4" t="s">
-        <v>5</v>
+        <v>104</v>
       </c>
     </row>
     <row r="35" spans="2:11" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Feat: add roles table
</commit_message>
<xml_diff>
--- a/proyecto/iteración-2/docs/modelos/modelo-relacional.xlsx
+++ b/proyecto/iteración-2/docs/modelos/modelo-relacional.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zejiran/hack/uniandes/B-03/proyecto/iteración-2/docs/modelos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FBAB829-516C-0B4F-BEFA-F7C1EA4F5D92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72B0E0A7-31DB-4449-A3A2-66500F801E35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6080" yWindow="21600" windowWidth="25600" windowHeight="16000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plantilla Relación" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="108">
   <si>
     <t>NN</t>
   </si>
@@ -247,9 +247,6 @@
     <t>CK in ('PersonaNatural', 'Empresa')</t>
   </si>
   <si>
-    <t>NN, CK in ('Administrador', 'GerenteGeneral', 'GerenteSucursal', 'Operador', 'Cajero', 'Cliente')</t>
-  </si>
-  <si>
     <t>NN, FK Contenedor.id</t>
   </si>
   <si>
@@ -350,6 +347,18 @@
   </si>
   <si>
     <t>DD, CK between 0 and 5</t>
+  </si>
+  <si>
+    <t>Rol</t>
+  </si>
+  <si>
+    <t>NN, FK Rol.id</t>
+  </si>
+  <si>
+    <t>idRol</t>
+  </si>
+  <si>
+    <t>ND, NN</t>
   </si>
 </sst>
 </file>
@@ -886,8 +895,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:L45"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="75" zoomScaleNormal="135" workbookViewId="0">
-      <selection activeCell="K29" sqref="K29"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B9" zoomScale="75" zoomScaleNormal="135" workbookViewId="0">
+      <selection activeCell="K31" sqref="K31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -934,19 +943,19 @@
         <v>45</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="J3" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="K3" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="L3" s="8" t="s">
         <v>88</v>
-      </c>
-      <c r="L3" s="8" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="4" spans="2:12" s="5" customFormat="1" ht="51" x14ac:dyDescent="0.2">
@@ -967,19 +976,19 @@
       </c>
       <c r="G4" s="9"/>
       <c r="H4" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="I4" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="I4" s="12" t="s">
-        <v>81</v>
-      </c>
       <c r="J4" s="9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="K4" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="L4" s="9" t="s">
         <v>86</v>
-      </c>
-      <c r="L4" s="9" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.2">
@@ -1014,13 +1023,13 @@
         <v>40</v>
       </c>
       <c r="E8" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="F8" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="F8" s="3" t="s">
-        <v>83</v>
-      </c>
       <c r="G8" s="8" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I8" s="3" t="s">
         <v>2</v>
@@ -1043,7 +1052,7 @@
         <v>5</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>0</v>
@@ -1052,13 +1061,13 @@
         <v>0</v>
       </c>
       <c r="G9" s="12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I9" s="4" t="s">
         <v>4</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="K9" s="4" t="s">
         <v>0</v>
@@ -1081,7 +1090,7 @@
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H12" s="1" t="s">
         <v>9</v>
@@ -1148,7 +1157,7 @@
         <v>0</v>
       </c>
       <c r="L14" s="9" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.2">
@@ -1168,10 +1177,10 @@
         <v>8</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="18" spans="2:12" x14ac:dyDescent="0.2">
@@ -1188,22 +1197,22 @@
         <v>34</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H18" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="I18" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="J18" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="I18" s="8" t="s">
+      <c r="K18" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="L18" s="3" t="s">
         <v>97</v>
-      </c>
-      <c r="J18" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="K18" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="L18" s="3" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="19" spans="2:12" ht="34" x14ac:dyDescent="0.2">
@@ -1218,19 +1227,19 @@
         <v>67</v>
       </c>
       <c r="F19" s="12" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H19" s="12" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I19" s="12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="K19" s="12" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="L19" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="20" spans="2:12" x14ac:dyDescent="0.2">
@@ -1269,7 +1278,7 @@
         <v>21</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>22</v>
+        <v>106</v>
       </c>
       <c r="I23" s="3" t="s">
         <v>23</v>
@@ -1278,10 +1287,10 @@
         <v>24</v>
       </c>
       <c r="K23" s="8" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="24" spans="2:12" ht="68" x14ac:dyDescent="0.2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="24" spans="2:12" ht="17" x14ac:dyDescent="0.2">
       <c r="B24" s="4" t="s">
         <v>3</v>
       </c>
@@ -1301,12 +1310,12 @@
         <v>0</v>
       </c>
       <c r="H24" s="4" t="s">
-        <v>70</v>
+        <v>105</v>
       </c>
       <c r="I24" s="4"/>
       <c r="J24" s="4"/>
       <c r="K24" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="25" spans="2:12" x14ac:dyDescent="0.2">
@@ -1325,6 +1334,9 @@
       <c r="B27" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="J27" s="1" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="28" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B28" s="3" t="s">
@@ -1346,10 +1358,16 @@
         <v>49</v>
       </c>
       <c r="H28" s="3" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="29" spans="2:12" ht="51" x14ac:dyDescent="0.2">
+        <v>100</v>
+      </c>
+      <c r="J28" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K28" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="29" spans="2:12" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B29" s="4" t="s">
         <v>4</v>
       </c>
@@ -1367,7 +1385,13 @@
       </c>
       <c r="G29" s="9"/>
       <c r="H29" s="12" t="s">
-        <v>81</v>
+        <v>80</v>
+      </c>
+      <c r="J29" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="K29" s="4" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="30" spans="2:12" x14ac:dyDescent="0.2">
@@ -1378,6 +1402,8 @@
       <c r="F30" s="10"/>
       <c r="G30" s="10"/>
       <c r="H30" s="6"/>
+      <c r="J30" s="6"/>
+      <c r="K30" s="7"/>
     </row>
     <row r="32" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B32" s="1" t="s">
@@ -1440,7 +1466,7 @@
         <v>0</v>
       </c>
       <c r="K34" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="35" spans="2:11" x14ac:dyDescent="0.2">
@@ -1482,7 +1508,7 @@
         <v>61</v>
       </c>
       <c r="I38" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="39" spans="2:11" ht="51" x14ac:dyDescent="0.2">
@@ -1506,7 +1532,7 @@
         <v>63</v>
       </c>
       <c r="I39" s="12" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="40" spans="2:11" x14ac:dyDescent="0.2">
@@ -1524,7 +1550,7 @@
         <v>15</v>
       </c>
       <c r="H42" s="13" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I42" s="11"/>
     </row>
@@ -1539,16 +1565,16 @@
         <v>54</v>
       </c>
       <c r="E43" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="F43" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="H43" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="I43" s="8" t="s">
         <v>77</v>
-      </c>
-      <c r="F43" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="H43" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="I43" s="8" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="44" spans="2:11" ht="17" x14ac:dyDescent="0.2">
@@ -1558,16 +1584,16 @@
       <c r="C44" s="4"/>
       <c r="D44" s="4"/>
       <c r="E44" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F44" s="9" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H44" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I44" s="12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="45" spans="2:11" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Fix: add new properties at promocion and compra
</commit_message>
<xml_diff>
--- a/proyecto/iteración-2/docs/modelos/modelo-relacional.xlsx
+++ b/proyecto/iteración-2/docs/modelos/modelo-relacional.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zejiran/hack/uniandes/B-03/proyecto/iteración-2/docs/modelos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72B0E0A7-31DB-4449-A3A2-66500F801E35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BF8079B-4535-3B45-9A84-8C22CC1D3188}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6080" yWindow="21600" windowWidth="25600" windowHeight="16000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plantilla Relación" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="109">
   <si>
     <t>NN</t>
   </si>
@@ -343,9 +343,6 @@
     <t>idCompra</t>
   </si>
   <si>
-    <t>O</t>
-  </si>
-  <si>
     <t>DD, CK between 0 and 5</t>
   </si>
   <si>
@@ -359,6 +356,12 @@
   </si>
   <si>
     <t>ND, NN</t>
+  </si>
+  <si>
+    <t>cantUnidadesCompradas</t>
+  </si>
+  <si>
+    <t>cantUnidadesDisponibles</t>
   </si>
 </sst>
 </file>
@@ -893,10 +896,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:L45"/>
+  <dimension ref="B2:M45"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B9" zoomScale="75" zoomScaleNormal="135" workbookViewId="0">
-      <selection activeCell="K31" sqref="K31"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScale="75" zoomScaleNormal="135" workbookViewId="0">
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -910,7 +913,7 @@
     <col min="7" max="7" width="21" style="2" customWidth="1"/>
     <col min="8" max="8" width="29.5" style="2" customWidth="1"/>
     <col min="9" max="9" width="27" style="2" customWidth="1"/>
-    <col min="10" max="10" width="20.83203125" style="2" customWidth="1"/>
+    <col min="10" max="10" width="23" style="2" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="22.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="28.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="23.83203125" style="2" customWidth="1"/>
@@ -918,12 +921,12 @@
     <col min="15" max="16384" width="8.6640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B3" s="3" t="s">
         <v>41</v>
       </c>
@@ -958,7 +961,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="4" spans="2:12" s="5" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:13" s="5" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="B4" s="4" t="s">
         <v>4</v>
       </c>
@@ -991,7 +994,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B5" s="6"/>
       <c r="C5" s="7"/>
       <c r="D5" s="6"/>
@@ -1004,15 +1007,15 @@
       <c r="K5" s="10"/>
       <c r="L5" s="10"/>
     </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I7" s="1" t="s">
+      <c r="J7" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B8" s="3" t="s">
         <v>2</v>
       </c>
@@ -1031,20 +1034,23 @@
       <c r="G8" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="I8" s="3" t="s">
+      <c r="H8" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="J8" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="J8" s="3" t="s">
+      <c r="K8" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="K8" s="3" t="s">
+      <c r="L8" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="L8" s="3" t="s">
+      <c r="M8" s="3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="2:12" ht="74" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:13" ht="74" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="4" t="s">
         <v>4</v>
       </c>
@@ -1063,32 +1069,36 @@
       <c r="G9" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="I9" s="4" t="s">
+      <c r="H9" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="J9" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="J9" s="4" t="s">
+      <c r="K9" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="K9" s="4" t="s">
-        <v>0</v>
-      </c>
       <c r="L9" s="4" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="M9" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B10" s="6"/>
       <c r="C10" s="7"/>
       <c r="D10" s="6"/>
       <c r="E10" s="6"/>
       <c r="F10" s="6"/>
       <c r="G10" s="15"/>
-      <c r="I10" s="6"/>
-      <c r="J10" s="7"/>
-      <c r="K10" s="6"/>
+      <c r="H10" s="15"/>
+      <c r="J10" s="6"/>
+      <c r="K10" s="7"/>
       <c r="L10" s="6"/>
-    </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="M10" s="6"/>
+    </row>
+    <row r="12" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
         <v>89</v>
       </c>
@@ -1096,7 +1106,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B13" s="3" t="s">
         <v>2</v>
       </c>
@@ -1128,7 +1138,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="2:12" ht="17" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:13" ht="17" x14ac:dyDescent="0.2">
       <c r="B14" s="4" t="s">
         <v>4</v>
       </c>
@@ -1160,7 +1170,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B15" s="6"/>
       <c r="C15" s="7"/>
       <c r="D15" s="6"/>
@@ -1172,18 +1182,18 @@
       <c r="K15" s="6"/>
       <c r="L15" s="10"/>
     </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B17" s="1" t="s">
         <v>8</v>
       </c>
       <c r="H17" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="K17" s="1" t="s">
+      <c r="L17" s="1" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B18" s="3" t="s">
         <v>2</v>
       </c>
@@ -1205,17 +1215,17 @@
       <c r="I18" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="J18" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="K18" s="3" t="s">
+      <c r="J18" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="L18" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="L18" s="3" t="s">
+      <c r="M18" s="3" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="19" spans="2:12" ht="34" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:13" ht="34" x14ac:dyDescent="0.2">
       <c r="B19" s="4" t="s">
         <v>4</v>
       </c>
@@ -1235,14 +1245,17 @@
       <c r="I19" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="K19" s="12" t="s">
+      <c r="J19" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="L19" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="L19" s="12" t="s">
+      <c r="M19" s="12" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B20" s="6"/>
       <c r="C20" s="7"/>
       <c r="D20" s="6"/>
@@ -1250,15 +1263,16 @@
       <c r="F20" s="6"/>
       <c r="H20" s="14"/>
       <c r="I20" s="15"/>
-      <c r="K20" s="6"/>
-      <c r="L20" s="7"/>
-    </row>
-    <row r="22" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="J20" s="15"/>
+      <c r="L20" s="6"/>
+      <c r="M20" s="7"/>
+    </row>
+    <row r="22" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B22" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="23" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B23" s="3" t="s">
         <v>17</v>
       </c>
@@ -1278,7 +1292,7 @@
         <v>21</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I23" s="3" t="s">
         <v>23</v>
@@ -1290,7 +1304,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="24" spans="2:12" ht="17" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:13" ht="17" x14ac:dyDescent="0.2">
       <c r="B24" s="4" t="s">
         <v>3</v>
       </c>
@@ -1310,7 +1324,7 @@
         <v>0</v>
       </c>
       <c r="H24" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="I24" s="4"/>
       <c r="J24" s="4"/>
@@ -1318,7 +1332,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="25" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B25" s="6"/>
       <c r="C25" s="7"/>
       <c r="D25" s="6"/>
@@ -1330,15 +1344,15 @@
       <c r="J25" s="6"/>
       <c r="K25" s="10"/>
     </row>
-    <row r="27" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B27" s="1" t="s">
         <v>12</v>
       </c>
       <c r="J27" s="1" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="28" spans="2:12" x14ac:dyDescent="0.2">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="28" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B28" s="3" t="s">
         <v>2</v>
       </c>
@@ -1367,7 +1381,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="29" spans="2:12" ht="72" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:13" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B29" s="4" t="s">
         <v>4</v>
       </c>
@@ -1391,10 +1405,10 @@
         <v>4</v>
       </c>
       <c r="K29" s="4" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="30" spans="2:12" x14ac:dyDescent="0.2">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="30" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B30" s="6"/>
       <c r="C30" s="7"/>
       <c r="D30" s="6"/>
@@ -1405,7 +1419,7 @@
       <c r="J30" s="6"/>
       <c r="K30" s="7"/>
     </row>
-    <row r="32" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B32" s="1" t="s">
         <v>13</v>
       </c>
@@ -1466,7 +1480,7 @@
         <v>0</v>
       </c>
       <c r="K34" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="35" spans="2:11" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Fix: update relational model
</commit_message>
<xml_diff>
--- a/proyecto/iteración-2/docs/modelos/modelo-relacional.xlsx
+++ b/proyecto/iteración-2/docs/modelos/modelo-relacional.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zejiran/hack/uniandes/B-03/proyecto/iteración-2/docs/modelos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BF8079B-4535-3B45-9A84-8C22CC1D3188}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C74D83CB-4BC0-9C45-AEF3-AF099BB0ABA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="110">
   <si>
     <t>NN</t>
   </si>
@@ -362,6 +362,9 @@
   </si>
   <si>
     <t>cantUnidadesDisponibles</t>
+  </si>
+  <si>
+    <t>fechaCompra</t>
   </si>
 </sst>
 </file>
@@ -899,7 +902,7 @@
   <dimension ref="B2:M45"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScale="75" zoomScaleNormal="135" workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1182,18 +1185,15 @@
       <c r="K15" s="6"/>
       <c r="L15" s="10"/>
     </row>
-    <row r="17" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B17" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H17" s="1" t="s">
+      <c r="I17" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="L17" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="18" spans="2:13" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B18" s="3" t="s">
         <v>2</v>
       </c>
@@ -1209,23 +1209,20 @@
       <c r="F18" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="H18" s="8" t="s">
+      <c r="G18" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="I18" s="8" t="s">
         <v>101</v>
       </c>
-      <c r="I18" s="8" t="s">
+      <c r="J18" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="J18" s="8" t="s">
+      <c r="K18" s="8" t="s">
         <v>107</v>
       </c>
-      <c r="L18" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="M18" s="3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="19" spans="2:13" ht="34" x14ac:dyDescent="0.2">
+    </row>
+    <row r="19" spans="2:11" ht="34" x14ac:dyDescent="0.2">
       <c r="B19" s="4" t="s">
         <v>4</v>
       </c>
@@ -1239,40 +1236,36 @@
       <c r="F19" s="12" t="s">
         <v>84</v>
       </c>
-      <c r="H19" s="12" t="s">
+      <c r="G19" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="I19" s="12" t="s">
         <v>94</v>
       </c>
-      <c r="I19" s="12" t="s">
+      <c r="J19" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="J19" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="L19" s="12" t="s">
-        <v>73</v>
-      </c>
-      <c r="M19" s="12" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="20" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="K19" s="12" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B20" s="6"/>
       <c r="C20" s="7"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
-      <c r="H20" s="14"/>
-      <c r="I20" s="15"/>
+      <c r="G20" s="6"/>
+      <c r="I20" s="14"/>
       <c r="J20" s="15"/>
-      <c r="L20" s="6"/>
-      <c r="M20" s="7"/>
-    </row>
-    <row r="22" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="K20" s="15"/>
+    </row>
+    <row r="22" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B22" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="23" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B23" s="3" t="s">
         <v>17</v>
       </c>
@@ -1304,7 +1297,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="24" spans="2:13" ht="17" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:11" ht="17" x14ac:dyDescent="0.2">
       <c r="B24" s="4" t="s">
         <v>3</v>
       </c>
@@ -1332,7 +1325,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="25" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B25" s="6"/>
       <c r="C25" s="7"/>
       <c r="D25" s="6"/>
@@ -1344,7 +1337,7 @@
       <c r="J25" s="6"/>
       <c r="K25" s="10"/>
     </row>
-    <row r="27" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B27" s="1" t="s">
         <v>12</v>
       </c>
@@ -1352,7 +1345,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="28" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B28" s="3" t="s">
         <v>2</v>
       </c>
@@ -1381,7 +1374,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="29" spans="2:13" ht="72" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:11" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B29" s="4" t="s">
         <v>4</v>
       </c>
@@ -1408,7 +1401,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="30" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B30" s="6"/>
       <c r="C30" s="7"/>
       <c r="D30" s="6"/>
@@ -1419,7 +1412,7 @@
       <c r="J30" s="6"/>
       <c r="K30" s="7"/>
     </row>
-    <row r="32" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B32" s="1" t="s">
         <v>13</v>
       </c>
@@ -1427,7 +1420,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="33" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B33" s="3" t="s">
         <v>2</v>
       </c>
@@ -1456,7 +1449,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="34" spans="2:11" ht="17" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:12" ht="17" x14ac:dyDescent="0.2">
       <c r="B34" s="12" t="s">
         <v>4</v>
       </c>
@@ -1483,7 +1476,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="35" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B35" s="6"/>
       <c r="C35" s="7"/>
       <c r="D35" s="6"/>
@@ -1494,12 +1487,15 @@
       <c r="J35" s="7"/>
       <c r="K35" s="6"/>
     </row>
-    <row r="37" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B37" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="38" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="K37" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="38" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B38" s="3" t="s">
         <v>2</v>
       </c>
@@ -1524,8 +1520,14 @@
       <c r="I38" s="3" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="39" spans="2:11" ht="51" x14ac:dyDescent="0.2">
+      <c r="K38" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="L38" s="3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="39" spans="2:12" ht="51" x14ac:dyDescent="0.2">
       <c r="B39" s="4" t="s">
         <v>4</v>
       </c>
@@ -1548,8 +1550,14 @@
       <c r="I39" s="12" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="40" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="K39" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="L39" s="12" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="40" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B40" s="6"/>
       <c r="C40" s="7"/>
       <c r="D40" s="6"/>
@@ -1558,8 +1566,10 @@
       <c r="G40" s="10"/>
       <c r="H40" s="10"/>
       <c r="I40" s="6"/>
-    </row>
-    <row r="42" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="K40" s="6"/>
+      <c r="L40" s="7"/>
+    </row>
+    <row r="42" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B42" s="1" t="s">
         <v>15</v>
       </c>
@@ -1568,7 +1578,7 @@
       </c>
       <c r="I42" s="11"/>
     </row>
-    <row r="43" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B43" s="3" t="s">
         <v>2</v>
       </c>
@@ -1591,7 +1601,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="44" spans="2:11" ht="17" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:12" ht="17" x14ac:dyDescent="0.2">
       <c r="B44" s="12" t="s">
         <v>4</v>
       </c>
@@ -1610,7 +1620,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="45" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B45" s="6"/>
       <c r="C45" s="7"/>
       <c r="D45" s="6"/>

</xml_diff>

<commit_message>
Fix: add new property to promocion
</commit_message>
<xml_diff>
--- a/proyecto/iteración-2/docs/modelos/modelo-relacional.xlsx
+++ b/proyecto/iteración-2/docs/modelos/modelo-relacional.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zejiran/hack/uniandes/B-03/proyecto/iteración-2/docs/modelos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C74D83CB-4BC0-9C45-AEF3-AF099BB0ABA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC999FF9-2B4F-544B-95A6-0B493EDA7299}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plantilla Relación" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="111">
   <si>
     <t>NN</t>
   </si>
@@ -365,6 +365,9 @@
   </si>
   <si>
     <t>fechaCompra</t>
+  </si>
+  <si>
+    <t>totalUnidadesOfrecidas</t>
   </si>
 </sst>
 </file>
@@ -899,10 +902,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:M45"/>
+  <dimension ref="B2:N45"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScale="75" zoomScaleNormal="135" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="63" zoomScaleNormal="135" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -924,12 +927,12 @@
     <col min="15" max="16384" width="8.6640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B3" s="3" t="s">
         <v>41</v>
       </c>
@@ -964,7 +967,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="4" spans="2:13" s="5" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:14" s="5" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="B4" s="4" t="s">
         <v>4</v>
       </c>
@@ -997,7 +1000,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="5" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B5" s="6"/>
       <c r="C5" s="7"/>
       <c r="D5" s="6"/>
@@ -1010,15 +1013,15 @@
       <c r="K5" s="10"/>
       <c r="L5" s="10"/>
     </row>
-    <row r="7" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J7" s="1" t="s">
+      <c r="K7" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B8" s="3" t="s">
         <v>2</v>
       </c>
@@ -1040,20 +1043,23 @@
       <c r="H8" s="8" t="s">
         <v>108</v>
       </c>
-      <c r="J8" s="3" t="s">
+      <c r="I8" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="K8" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="K8" s="3" t="s">
+      <c r="L8" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="L8" s="3" t="s">
+      <c r="M8" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="M8" s="3" t="s">
+      <c r="N8" s="3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="2:13" ht="74" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:14" ht="74" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="4" t="s">
         <v>4</v>
       </c>
@@ -1075,20 +1081,23 @@
       <c r="H9" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="J9" s="4" t="s">
+      <c r="I9" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="K9" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="K9" s="4" t="s">
+      <c r="L9" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="L9" s="4" t="s">
-        <v>0</v>
-      </c>
       <c r="M9" s="4" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="N9" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B10" s="6"/>
       <c r="C10" s="7"/>
       <c r="D10" s="6"/>
@@ -1096,12 +1105,13 @@
       <c r="F10" s="6"/>
       <c r="G10" s="15"/>
       <c r="H10" s="15"/>
-      <c r="J10" s="6"/>
-      <c r="K10" s="7"/>
-      <c r="L10" s="6"/>
+      <c r="I10" s="15"/>
+      <c r="K10" s="6"/>
+      <c r="L10" s="7"/>
       <c r="M10" s="6"/>
-    </row>
-    <row r="12" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="N10" s="6"/>
+    </row>
+    <row r="12" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
         <v>89</v>
       </c>
@@ -1109,7 +1119,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B13" s="3" t="s">
         <v>2</v>
       </c>
@@ -1141,7 +1151,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="2:13" ht="17" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:14" ht="17" x14ac:dyDescent="0.2">
       <c r="B14" s="4" t="s">
         <v>4</v>
       </c>
@@ -1173,7 +1183,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="15" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B15" s="6"/>
       <c r="C15" s="7"/>
       <c r="D15" s="6"/>
@@ -1449,7 +1459,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="34" spans="2:12" ht="17" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:12" ht="54" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B34" s="12" t="s">
         <v>4</v>
       </c>
@@ -1601,7 +1611,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="44" spans="2:12" ht="17" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:12" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B44" s="12" t="s">
         <v>4</v>
       </c>

</xml_diff>